<commit_message>
new feature: if alg contains 💩 emoji, then `difficult` is set to True
</commit_message>
<xml_diff>
--- a/Files_tests/test_algs.xlsx
+++ b/Files_tests/test_algs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>UB (A)</t>
   </si>
@@ -34,10 +34,10 @@
     <t>ventarowy U perm</t>
   </si>
   <si>
-    <t>[U perm]</t>
-  </si>
-  <si>
-    <t/>
+    <t>U' [U perm] 💩</t>
+  </si>
+  <si>
+    <t>[U perm] 💩</t>
   </si>
   <si>
     <t>U [U perm]</t>
@@ -96,16 +96,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -420,12 +423,12 @@
   <cols>
     <col min="1" max="1" style="4" width="13.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -440,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -451,24 +454,22 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -476,23 +477,23 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>